<commit_message>
creating the front-end user inputs and js to create inputs and alter min/max
</commit_message>
<xml_diff>
--- a/Situation_room_test.xlsx
+++ b/Situation_room_test.xlsx
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794917FB-95D6-4D82-9D04-1385F0D9843E}">
   <dimension ref="B2:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>